<commit_message>
Se valida la creación del grafico 2
</commit_message>
<xml_diff>
--- a/Auto-Excel/InventarioV3.xlsx
+++ b/Auto-Excel/InventarioV3.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Inventario principal" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Reporte 2025-04-15" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Reporte 2025-04-16" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -282,6 +282,59 @@
 </chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="10"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Distribución de categorías</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <pieChart>
+        <varyColors val="1"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Inventario principal'!$A$2:$A$6</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Inventario principal'!$D$2:$D$6</f>
+            </numRef>
+          </val>
+        </ser>
+        <firstSliceAng val="0"/>
+      </pieChart>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
@@ -301,6 +354,28 @@
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>17</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="2" name="Chart 2"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>

</xml_diff>

<commit_message>
Se realizan pruebas de la tabla
</commit_message>
<xml_diff>
--- a/Auto-Excel/InventarioV3.xlsx
+++ b/Auto-Excel/InventarioV3.xlsx
@@ -384,6 +384,21 @@
 </wsDr>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TablaInventario" displayName="TablaInventario" ref="A1:F6" headerRowCount="1">
+  <autoFilter ref="A1:F6"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="ID"/>
+    <tableColumn id="2" name="Nombre"/>
+    <tableColumn id="3" name="Descripción"/>
+    <tableColumn id="4" name="Cantidad"/>
+    <tableColumn id="5" name="Precio Unitario"/>
+    <tableColumn id="6" name="Precio Total"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -844,6 +859,9 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Se finaliza la categorización de datos
</commit_message>
<xml_diff>
--- a/Auto-Excel/InventarioV3.xlsx
+++ b/Auto-Excel/InventarioV3.xlsx
@@ -857,6 +857,11 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B6" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" errorTitle="Error de validación" error="Por favor ingresar un producto correcto" type="list">
+      <formula1>"Producto A,Producto B,Producto C,Producto D,Producto E"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>